<commit_message>
Update report: Section Interrupt & Section General-Purpose I/O
</commit_message>
<xml_diff>
--- a/Report/Image/InterruptRoutineAddress.xlsx
+++ b/Report/Image/InterruptRoutineAddress.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Projects\Dual_core_Microcontroller\Image\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Projects\Dual_core_Microcontroller\Report\Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2C5A2BC-3ABD-4039-8F8F-F0913C20C523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6394FD-1601-4DE2-BBB5-41A9B97B7BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF8CC9C8-7238-44F2-A108-E2717A37B9C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Vector Number</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>Main Program</t>
+  </si>
+  <si>
+    <t>Sense Encode[6]</t>
+  </si>
+  <si>
+    <t>Sense Encode[5]</t>
+  </si>
+  <si>
+    <t>Sense Description</t>
+  </si>
+  <si>
+    <t>Rising Edge</t>
+  </si>
+  <si>
+    <t>Falling Edge</t>
+  </si>
+  <si>
+    <t>Change Level</t>
+  </si>
+  <si>
+    <t>Reserved</t>
   </si>
 </sst>
 </file>
@@ -131,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -142,6 +163,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF420485-CC0E-48DF-BE35-059FB6C85E12}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,6 +491,9 @@
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -524,7 +551,63 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update RTL: timer/counter's prescaler + Update Report: image
</commit_message>
<xml_diff>
--- a/Report/Image/InterruptRoutineAddress.xlsx
+++ b/Report/Image/InterruptRoutineAddress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Projects\Dual_core_Microcontroller\Report\Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6394FD-1601-4DE2-BBB5-41A9B97B7BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398B5E45-A742-4B7E-B53F-7411AD37DCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF8CC9C8-7238-44F2-A108-E2717A37B9C2}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{BF8CC9C8-7238-44F2-A108-E2717A37B9C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Vector Number</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>Reserved</t>
+  </si>
+  <si>
+    <t>Port Pin</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>Alternate Function</t>
+  </si>
+  <si>
+    <t>External Interrupt</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>Timer Limit Toggle Flag</t>
   </si>
 </sst>
 </file>
@@ -152,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -164,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,18 +501,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF420485-CC0E-48DF-BE35-059FB6C85E12}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="37.77734375" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
@@ -606,6 +628,44 @@
         <v>17</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>